<commit_message>
xpath logic and code restructure
</commit_message>
<xml_diff>
--- a/output/NY_TIMES_ARTICLES.xlsx
+++ b/output/NY_TIMES_ARTICLES.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,17 +491,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Taylor Swift’s Music Returns to TikTok Ahead of New Album</t>
+          <t>Golf’s Big Deal Veers Off Course</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Songs by the pop singer reappeared on TikTok despite the platform’s ongoing licensing dispute with Universal Music Group, which releases Swift’s music.</t>
+          <t>The Masters tournament should be all about sport, but the unresolved fight between the PGA Tour and LIV Golf looms over the competition.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>April 11</t>
+          <t>April 13</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -512,24 +512,24 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>images/11taylor-tiktok-wmbc-threeByTwoSmallAt2X.jpg</t>
+          <t>images/DB13-golf-jhfq-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>J. Cole Apologizes for Kendrick Lamar Diss Track</t>
+          <t>Taylor Swift’s Music Returns to TikTok Ahead of New Album</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>J. Cole also vowed to update the track, “7 Minute Drill,” or remove it from streaming services after it was featured on his new album, “Might Delete Later.”</t>
+          <t>Songs by the pop singer reappeared on TikTok despite the platform’s ongoing licensing dispute with Universal Music Group, which releases Swift’s music.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>April 8</t>
+          <t>April 11</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,33 +540,117 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>images/08xp-jcole-threeByTwoSmallAt2X.jpg</t>
+          <t>images/11taylor-tiktok-wmbc-threeByTwoSmallAt2X.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Richard Lyons, Former Business School Dean, Will Be U.C. Berkeley’s New Chancellor</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>The appointment comes as Berkeley and college campuses across the country are facing turmoil over free speech, racial and political diversity, and affordability.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>April 11</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>images/11californiatoday-ucb-threeByTwoSmallAt2X.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>36 Hours in Toronto</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Savor the diversity of this lakefront city though its hidden bars, small-but-fascinating museums and restaurants with dishes like jerk chicken chow mein and Hong Kong-style French toast.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>April 11</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>images/things-to-do-toronto-01-hwlf-threeByTwoSmallAt2X.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>J. Cole Apologizes for Kendrick Lamar Diss Track</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>J. Cole also vowed to update the track, “7 Minute Drill,” or remove it from streaming services after it was featured on his new album, “Might Delete Later.”</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>April 8</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>images/08xp-jcole-threeByTwoSmallAt2X.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Popcast (Deluxe): Listening to Beyoncé &amp; Future (and the Discourse)</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>How conversation about very specific aspects of the new albums “Cowboy Carter” and “We Don’t Trust You” can obscure talk of their musical quality.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>April 3</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>images/03popcast-deluxe-threeByTwoSmallAt2X.jpg</t>
         </is>

</xml_diff>